<commit_message>
Monday progress for 23.4
</commit_message>
<xml_diff>
--- a/StudyProgress.xlsx
+++ b/StudyProgress.xlsx
@@ -53347,8 +53347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53615,7 +53615,7 @@
         <v>0.5</v>
       </c>
       <c r="F2">
-        <f>SUM(H2:XFD2)</f>
+        <f t="shared" ref="F2:F33" si="0">SUM(H2:XFD2)</f>
         <v>0</v>
       </c>
       <c r="G2">
@@ -53631,15 +53631,15 @@
         <v>60</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E52" si="0">D3/60</f>
+        <f t="shared" ref="E3:E51" si="1">D3/60</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f>SUM(H3:XFD3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G52" si="1">E3-F3</f>
+        <f t="shared" ref="G3:G52" si="2">E3-F3</f>
         <v>1</v>
       </c>
     </row>
@@ -53651,15 +53651,15 @@
         <v>60</v>
       </c>
       <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <f>SUM(H4:XFD4)</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -53671,15 +53671,15 @@
         <v>120</v>
       </c>
       <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <f>SUM(H5:XFD5)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -53691,15 +53691,15 @@
         <v>60</v>
       </c>
       <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <f>SUM(H6:XFD6)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -53711,15 +53711,15 @@
         <v>60</v>
       </c>
       <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <f>SUM(H7:XFD7)</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -53731,15 +53731,15 @@
         <v>30</v>
       </c>
       <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <f>SUM(H8:XFD8)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -53758,15 +53758,15 @@
         <v>132</v>
       </c>
       <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F9">
-        <f>SUM(H9:XFD9)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -53785,15 +53785,15 @@
         <v>120</v>
       </c>
       <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <f>SUM(H10:XFD10)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -53812,15 +53812,15 @@
         <v>135</v>
       </c>
       <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="F11">
-        <f>SUM(H11:XFD11)</f>
         <v>1.5</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="H11">
@@ -53838,19 +53838,19 @@
         <v>22</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D51" si="2">C12*7</f>
+        <f t="shared" ref="D12:D51" si="3">C12*7</f>
         <v>154</v>
       </c>
       <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2.5666666666666669</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
-        <v>2.5666666666666669</v>
-      </c>
-      <c r="F12">
-        <f>SUM(H12:XFD12)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5666666666666669</v>
       </c>
     </row>
@@ -53865,19 +53865,19 @@
         <v>14</v>
       </c>
       <c r="D13">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.6333333333333333</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1.6333333333333333</v>
-      </c>
-      <c r="F13">
-        <f>SUM(H13:XFD13)</f>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
         <v>1.6333333333333333</v>
       </c>
     </row>
@@ -53892,19 +53892,19 @@
         <v>32</v>
       </c>
       <c r="D14">
+        <f t="shared" si="3"/>
+        <v>224</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>3.7333333333333334</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="2"/>
-        <v>224</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>3.7333333333333334</v>
-      </c>
-      <c r="F14">
-        <f>SUM(H14:XFD14)</f>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
         <v>3.7333333333333334</v>
       </c>
     </row>
@@ -53919,20 +53919,23 @@
         <v>33</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>231</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>3.85</v>
-      </c>
-      <c r="F15">
-        <f>SUM(H15:XFD15)</f>
-        <v>0</v>
-      </c>
-      <c r="G15">
         <f t="shared" si="1"/>
         <v>3.85</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>3.35</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.3">
@@ -53946,23 +53949,23 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="F16">
-        <f>SUM(H16:XFD16)</f>
-        <v>0</v>
-      </c>
-      <c r="G16">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -53973,23 +53976,26 @@
         <v>30</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="F17">
-        <f>SUM(H17:XFD17)</f>
-        <v>0</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="L17">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -54000,23 +54006,23 @@
         <v>31</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>3.6166666666666667</v>
-      </c>
-      <c r="F18">
-        <f>SUM(H18:XFD18)</f>
-        <v>0</v>
-      </c>
-      <c r="G18">
         <f t="shared" si="1"/>
         <v>3.6166666666666667</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>3.6166666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -54027,23 +54033,23 @@
         <v>32</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>3.7333333333333334</v>
-      </c>
-      <c r="F19">
-        <f>SUM(H19:XFD19)</f>
-        <v>0</v>
-      </c>
-      <c r="G19">
         <f t="shared" si="1"/>
         <v>3.7333333333333334</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>3.7333333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -54054,23 +54060,23 @@
         <v>7</v>
       </c>
       <c r="D20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0.81666666666666665</v>
-      </c>
-      <c r="F20">
-        <f>SUM(H20:XFD20)</f>
-        <v>0</v>
-      </c>
-      <c r="G20">
         <f t="shared" si="1"/>
         <v>0.81666666666666665</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0.81666666666666665</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -54081,23 +54087,23 @@
         <v>36</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>252</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="F21">
-        <f>SUM(H21:XFD21)</f>
-        <v>0</v>
-      </c>
-      <c r="G21">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -54108,23 +54114,23 @@
         <v>31</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>3.6166666666666667</v>
-      </c>
-      <c r="F22">
-        <f>SUM(H22:XFD22)</f>
-        <v>0</v>
-      </c>
-      <c r="G22">
         <f t="shared" si="1"/>
         <v>3.6166666666666667</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>3.6166666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -54135,23 +54141,23 @@
         <v>29</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>3.3833333333333333</v>
-      </c>
-      <c r="F23">
-        <f>SUM(H23:XFD23)</f>
-        <v>0</v>
-      </c>
-      <c r="G23">
         <f t="shared" si="1"/>
         <v>3.3833333333333333</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>3.3833333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -54162,23 +54168,23 @@
         <v>39</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>273</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-      <c r="F24">
-        <f>SUM(H24:XFD24)</f>
-        <v>0</v>
-      </c>
-      <c r="G24">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -54189,23 +54195,23 @@
         <v>34</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>238</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>3.9666666666666668</v>
-      </c>
-      <c r="F25">
-        <f>SUM(H25:XFD25)</f>
-        <v>0</v>
-      </c>
-      <c r="G25">
         <f t="shared" si="1"/>
         <v>3.9666666666666668</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>3.9666666666666668</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -54216,23 +54222,23 @@
         <v>5</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="F26">
-        <f>SUM(H26:XFD26)</f>
-        <v>0</v>
-      </c>
-      <c r="G26">
         <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -54243,23 +54249,23 @@
         <v>8</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="F27">
-        <f>SUM(H27:XFD27)</f>
-        <v>0</v>
-      </c>
-      <c r="G27">
         <f t="shared" si="1"/>
         <v>0.93333333333333335</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -54270,23 +54276,23 @@
         <v>31</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>3.6166666666666667</v>
-      </c>
-      <c r="F28">
-        <f>SUM(H28:XFD28)</f>
-        <v>0</v>
-      </c>
-      <c r="G28">
         <f t="shared" si="1"/>
         <v>3.6166666666666667</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>3.6166666666666667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -54297,23 +54303,23 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="F29">
-        <f>SUM(H29:XFD29)</f>
-        <v>0</v>
-      </c>
-      <c r="G29">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>70</v>
       </c>
@@ -54324,23 +54330,23 @@
         <v>31</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>3.6166666666666667</v>
-      </c>
-      <c r="F30">
-        <f>SUM(H30:XFD30)</f>
-        <v>0</v>
-      </c>
-      <c r="G30">
         <f t="shared" si="1"/>
         <v>3.6166666666666667</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>3.6166666666666667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>70</v>
       </c>
@@ -54351,23 +54357,23 @@
         <v>29</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>3.3833333333333333</v>
-      </c>
-      <c r="F31">
-        <f>SUM(H31:XFD31)</f>
-        <v>0</v>
-      </c>
-      <c r="G31">
         <f t="shared" si="1"/>
         <v>3.3833333333333333</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>3.3833333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -54378,19 +54384,19 @@
         <v>38</v>
       </c>
       <c r="D32">
+        <f t="shared" si="3"/>
+        <v>266</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>4.4333333333333336</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
         <f t="shared" si="2"/>
-        <v>266</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>4.4333333333333336</v>
-      </c>
-      <c r="F32">
-        <f>SUM(H32:XFD32)</f>
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="1"/>
         <v>4.4333333333333336</v>
       </c>
     </row>
@@ -54405,19 +54411,19 @@
         <v>9</v>
       </c>
       <c r="D33">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
         <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>1.05</v>
-      </c>
-      <c r="F33">
-        <f>SUM(H33:XFD33)</f>
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
     </row>
@@ -54432,19 +54438,19 @@
         <v>21</v>
       </c>
       <c r="D34">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F51" si="4">SUM(H34:XFD34)</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
         <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="F34">
-        <f>SUM(H34:XFD34)</f>
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="1"/>
         <v>2.4500000000000002</v>
       </c>
     </row>
@@ -54459,19 +54465,19 @@
         <v>29</v>
       </c>
       <c r="D35">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>3.3833333333333333</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="2"/>
-        <v>203</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>3.3833333333333333</v>
-      </c>
-      <c r="F35">
-        <f>SUM(H35:XFD35)</f>
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="1"/>
         <v>3.3833333333333333</v>
       </c>
     </row>
@@ -54486,19 +54492,19 @@
         <v>25</v>
       </c>
       <c r="D36">
+        <f t="shared" si="3"/>
+        <v>175</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
         <f t="shared" si="2"/>
-        <v>175</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>2.9166666666666665</v>
-      </c>
-      <c r="F36">
-        <f>SUM(H36:XFD36)</f>
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="1"/>
         <v>2.9166666666666665</v>
       </c>
     </row>
@@ -54513,19 +54519,19 @@
         <v>13</v>
       </c>
       <c r="D37">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
         <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>1.5166666666666666</v>
-      </c>
-      <c r="F37">
-        <f>SUM(H37:XFD37)</f>
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="1"/>
         <v>1.5166666666666666</v>
       </c>
     </row>
@@ -54540,19 +54546,19 @@
         <v>30</v>
       </c>
       <c r="D38">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
         <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="F38">
-        <f>SUM(H38:XFD38)</f>
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
@@ -54567,19 +54573,19 @@
         <v>10</v>
       </c>
       <c r="D39">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="F39">
-        <f>SUM(H39:XFD39)</f>
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
     </row>
@@ -54594,19 +54600,19 @@
         <v>11</v>
       </c>
       <c r="D40">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.2833333333333334</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>1.2833333333333334</v>
-      </c>
-      <c r="F40">
-        <f>SUM(H40:XFD40)</f>
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="1"/>
         <v>1.2833333333333334</v>
       </c>
     </row>
@@ -54621,19 +54627,19 @@
         <v>14</v>
       </c>
       <c r="D41">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1.6333333333333333</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>1.6333333333333333</v>
-      </c>
-      <c r="F41">
-        <f>SUM(H41:XFD41)</f>
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="1"/>
         <v>1.6333333333333333</v>
       </c>
     </row>
@@ -54648,19 +54654,19 @@
         <v>15</v>
       </c>
       <c r="D42">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
-      </c>
-      <c r="F42">
-        <f>SUM(H42:XFD42)</f>
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -54675,19 +54681,19 @@
         <v>8</v>
       </c>
       <c r="D43">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="F43">
-        <f>SUM(H43:XFD43)</f>
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="1"/>
         <v>0.93333333333333335</v>
       </c>
     </row>
@@ -54702,19 +54708,19 @@
         <v>9</v>
       </c>
       <c r="D44">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>1.05</v>
-      </c>
-      <c r="F44">
-        <f>SUM(H44:XFD44)</f>
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
     </row>
@@ -54729,19 +54735,19 @@
         <v>4</v>
       </c>
       <c r="D45">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="F45">
-        <f>SUM(H45:XFD45)</f>
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="1"/>
         <v>0.46666666666666667</v>
       </c>
     </row>
@@ -54756,19 +54762,19 @@
         <v>24</v>
       </c>
       <c r="D46">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
         <f t="shared" si="2"/>
-        <v>168</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="F46">
-        <f>SUM(H46:XFD46)</f>
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
@@ -54783,19 +54789,19 @@
         <v>40</v>
       </c>
       <c r="D47">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="2"/>
-        <v>280</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="F47">
-        <f>SUM(H47:XFD47)</f>
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
     </row>
@@ -54810,19 +54816,19 @@
         <v>24</v>
       </c>
       <c r="D48">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="2"/>
-        <v>168</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="F48">
-        <f>SUM(H48:XFD48)</f>
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
@@ -54837,19 +54843,19 @@
         <v>28</v>
       </c>
       <c r="D49">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>3.2666666666666666</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49">
         <f t="shared" si="2"/>
-        <v>196</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
-        <v>3.2666666666666666</v>
-      </c>
-      <c r="F49">
-        <f>SUM(H49:XFD49)</f>
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="1"/>
         <v>3.2666666666666666</v>
       </c>
     </row>
@@ -54864,19 +54870,19 @@
         <v>22</v>
       </c>
       <c r="D50">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>2.5666666666666669</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G50">
         <f t="shared" si="2"/>
-        <v>154</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
-        <v>2.5666666666666669</v>
-      </c>
-      <c r="F50">
-        <f>SUM(H50:XFD50)</f>
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="1"/>
         <v>2.5666666666666669</v>
       </c>
     </row>
@@ -54891,19 +54897,19 @@
         <v>9</v>
       </c>
       <c r="D51">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
         <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>1.05</v>
-      </c>
-      <c r="F51">
-        <f>SUM(H51:XFD51)</f>
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
     </row>
@@ -54922,166 +54928,166 @@
       </c>
       <c r="F52">
         <f>SUM(F2:F51)</f>
-        <v>1.5</v>
+        <v>3.25</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
-        <v>114.26666666666667</v>
+        <f t="shared" si="2"/>
+        <v>112.51666666666667</v>
       </c>
       <c r="H52">
         <f>SUM(H2:H51)</f>
         <v>1.5</v>
       </c>
       <c r="I52">
-        <f t="shared" ref="I52:AT52" si="3">SUM(I2:I51)</f>
+        <f t="shared" ref="I52:AT52" si="5">SUM(I2:I51)</f>
         <v>0</v>
       </c>
       <c r="J52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
+        <v>1.75</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M52">
-        <f t="shared" si="3"/>
+      <c r="N52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N52">
-        <f t="shared" si="3"/>
+      <c r="O52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O52">
-        <f t="shared" si="3"/>
+      <c r="P52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P52">
-        <f t="shared" si="3"/>
+      <c r="Q52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q52">
-        <f t="shared" si="3"/>
+      <c r="R52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R52">
-        <f t="shared" si="3"/>
+      <c r="S52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S52">
-        <f t="shared" si="3"/>
+      <c r="T52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T52">
-        <f t="shared" si="3"/>
+      <c r="U52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U52">
-        <f t="shared" si="3"/>
+      <c r="V52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V52">
-        <f t="shared" si="3"/>
+      <c r="W52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W52">
-        <f t="shared" si="3"/>
+      <c r="X52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="X52">
-        <f t="shared" si="3"/>
+      <c r="Y52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Y52">
-        <f t="shared" si="3"/>
+      <c r="Z52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z52">
-        <f t="shared" si="3"/>
+      <c r="AA52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AA52">
-        <f t="shared" si="3"/>
+      <c r="AB52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB52">
-        <f t="shared" si="3"/>
+      <c r="AC52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AC52">
-        <f t="shared" si="3"/>
+      <c r="AD52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD52">
-        <f t="shared" si="3"/>
+      <c r="AE52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE52">
-        <f t="shared" si="3"/>
+      <c r="AF52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AF52">
-        <f t="shared" si="3"/>
+      <c r="AG52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AG52">
-        <f t="shared" si="3"/>
+      <c r="AH52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AH52">
-        <f t="shared" si="3"/>
+      <c r="AI52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AI52">
-        <f t="shared" si="3"/>
+      <c r="AJ52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AJ52">
-        <f t="shared" si="3"/>
+      <c r="AK52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AK52">
-        <f t="shared" si="3"/>
+      <c r="AL52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AL52">
-        <f t="shared" si="3"/>
+      <c r="AM52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AM52">
-        <f t="shared" si="3"/>
+      <c r="AN52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AN52">
-        <f t="shared" si="3"/>
+      <c r="AO52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO52">
-        <f t="shared" si="3"/>
+      <c r="AP52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AP52">
-        <f t="shared" si="3"/>
+      <c r="AQ52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AQ52">
-        <f t="shared" si="3"/>
+      <c r="AR52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR52">
-        <f t="shared" si="3"/>
+      <c r="AS52">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AS52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="AT52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new updates for concept checks
</commit_message>
<xml_diff>
--- a/StudyProgress.xlsx
+++ b/StudyProgress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="18180" windowHeight="7152" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="18180" windowHeight="7152" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RawQuestionDB" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3727" uniqueCount="124">
   <si>
     <t>Code</t>
   </si>
@@ -398,6 +398,45 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>liquidity premium, fwd rate and expected</t>
+  </si>
+  <si>
+    <t>liquidity theory</t>
+  </si>
+  <si>
+    <t>NC***</t>
+  </si>
+  <si>
+    <t>Human capital assets, labor intensive firm</t>
+  </si>
+  <si>
+    <t>Long formula account for labor income</t>
+  </si>
+  <si>
+    <t>extra market source of risks</t>
+  </si>
+  <si>
+    <t>liquidity beta</t>
+  </si>
+  <si>
+    <t>B313</t>
+  </si>
+  <si>
+    <t>sensitivity of return to market iliquidity</t>
+  </si>
+  <si>
+    <t>problem of testing market is efficient</t>
+  </si>
+  <si>
+    <t>Consumption CAPM assumption</t>
+  </si>
+  <si>
+    <t>allocate between current consumption and savings to support future</t>
+  </si>
+  <si>
+    <t>Shortcoming of CCAPM</t>
+  </si>
 </sst>
 </file>
 
@@ -11924,6 +11963,7 @@
   <autoFilter ref="A1:J719">
     <filterColumn colId="2">
       <filters>
+        <filter val="BKM15/Hull4"/>
         <filter val="BKM9"/>
       </filters>
     </filterColumn>
@@ -12236,7 +12276,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:R719"/>
   <sheetViews>
-    <sheetView topLeftCell="A264" workbookViewId="0">
+    <sheetView topLeftCell="A300" workbookViewId="0">
       <selection activeCell="J211" sqref="J211"/>
     </sheetView>
   </sheetViews>
@@ -32407,8 +32447,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:R719"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J399" sqref="J399"/>
+    <sheetView topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="J442" sqref="J442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34538,7 +34578,7 @@
       <c r="I72" s="4"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF1268316</v>
@@ -34567,7 +34607,7 @@
       <c r="I73" s="4"/>
       <c r="J73" s="7"/>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF2269317</v>
@@ -34596,7 +34636,7 @@
       <c r="I74" s="4"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF3270318</v>
@@ -34625,7 +34665,7 @@
       <c r="I75" s="4"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF4271319</v>
@@ -34654,7 +34694,7 @@
       <c r="I76" s="4"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF5272320</v>
@@ -34683,7 +34723,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF6273321</v>
@@ -34712,7 +34752,7 @@
       <c r="I78" s="4"/>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF7274322</v>
@@ -34741,7 +34781,7 @@
       <c r="I79" s="4"/>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF8275323</v>
@@ -34770,7 +34810,7 @@
       <c r="I80" s="4"/>
       <c r="J80" s="7"/>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF9276324</v>
@@ -34799,7 +34839,7 @@
       <c r="I81" s="4"/>
       <c r="J81" s="7"/>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF10277325</v>
@@ -34828,7 +34868,7 @@
       <c r="I82" s="4"/>
       <c r="J82" s="7"/>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF11279327</v>
@@ -34857,7 +34897,7 @@
       <c r="I83" s="4"/>
       <c r="J83" s="7"/>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF12280328</v>
@@ -34886,7 +34926,7 @@
       <c r="I84" s="4"/>
       <c r="J84" s="7"/>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF13282330</v>
@@ -34915,7 +34955,7 @@
       <c r="I85" s="4"/>
       <c r="J85" s="7"/>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF14283331</v>
@@ -34944,7 +34984,7 @@
       <c r="I86" s="4"/>
       <c r="J86" s="7"/>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF15284332</v>
@@ -34973,7 +35013,7 @@
       <c r="I87" s="4"/>
       <c r="J87" s="7"/>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF16286334</v>
@@ -35002,7 +35042,7 @@
       <c r="I88" s="4"/>
       <c r="J88" s="7"/>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF17287335</v>
@@ -35031,7 +35071,7 @@
       <c r="I89" s="4"/>
       <c r="J89" s="7"/>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF18288336</v>
@@ -35060,7 +35100,7 @@
       <c r="I90" s="4"/>
       <c r="J90" s="7"/>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF19289337</v>
@@ -35089,7 +35129,7 @@
       <c r="I91" s="4"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF20290338</v>
@@ -35118,7 +35158,7 @@
       <c r="I92" s="4"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF21292340</v>
@@ -35147,7 +35187,7 @@
       <c r="I93" s="4"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF22293341</v>
@@ -35176,7 +35216,7 @@
       <c r="I94" s="4"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF23295343</v>
@@ -35205,7 +35245,7 @@
       <c r="I95" s="4"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF24296344</v>
@@ -35234,7 +35274,7 @@
       <c r="I96" s="4"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF25297345</v>
@@ -35263,7 +35303,7 @@
       <c r="I97" s="4"/>
       <c r="J97" s="7"/>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF26298346</v>
@@ -35292,7 +35332,7 @@
       <c r="I98" s="4"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF27299347</v>
@@ -35321,7 +35361,7 @@
       <c r="I99" s="4"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF282100348</v>
@@ -35350,7 +35390,7 @@
       <c r="I100" s="4"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF292101349</v>
@@ -35379,7 +35419,7 @@
       <c r="I101" s="4"/>
       <c r="J101" s="7"/>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF302102350</v>
@@ -35408,7 +35448,7 @@
       <c r="I102" s="4"/>
       <c r="J102" s="7"/>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF312104352</v>
@@ -35437,7 +35477,7 @@
       <c r="I103" s="4"/>
       <c r="J103" s="7"/>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="str">
         <f t="shared" si="1"/>
         <v>GoldfarbQandAGF322106354</v>
@@ -39874,7 +39914,7 @@
       <c r="I256" s="4"/>
       <c r="J256" s="7"/>
     </row>
-    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" s="7" t="str">
         <f t="shared" si="3"/>
         <v>SectionB_SampleQTIA1213</v>
@@ -39903,7 +39943,7 @@
       <c r="I257" s="4"/>
       <c r="J257" s="7"/>
     </row>
-    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" s="7" t="str">
         <f t="shared" si="3"/>
         <v>SectionB_SampleQTIA2213</v>
@@ -39932,7 +39972,7 @@
       <c r="I258" s="4"/>
       <c r="J258" s="7"/>
     </row>
-    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" s="7" t="str">
         <f t="shared" ref="A259:A322" si="4">B259&amp;D259&amp;E259&amp;F259&amp;G259&amp;H259</f>
         <v>SectionB_SampleQTIA3214</v>
@@ -39961,7 +40001,7 @@
       <c r="I259" s="4"/>
       <c r="J259" s="7"/>
     </row>
-    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" s="7" t="str">
         <f t="shared" si="4"/>
         <v>SectionB_SampleQTIA4214</v>
@@ -39990,7 +40030,7 @@
       <c r="I260" s="4"/>
       <c r="J260" s="7"/>
     </row>
-    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" s="7" t="str">
         <f t="shared" si="4"/>
         <v>SectionB_SampleQTIA5225</v>
@@ -40019,7 +40059,7 @@
       <c r="I261" s="4"/>
       <c r="J261" s="7"/>
     </row>
-    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" s="7" t="str">
         <f t="shared" si="4"/>
         <v>SectionB_SampleQTIA6225</v>
@@ -40048,7 +40088,7 @@
       <c r="I262" s="4"/>
       <c r="J262" s="7"/>
     </row>
-    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" s="7" t="str">
         <f t="shared" si="4"/>
         <v>SectionB_SampleQTIA7226</v>
@@ -45260,7 +45300,7 @@
       <c r="I439" s="4"/>
       <c r="J439" s="7"/>
     </row>
-    <row r="440" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A440" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2000162111</v>
@@ -45289,7 +45329,7 @@
       <c r="I440" s="4"/>
       <c r="J440" s="7"/>
     </row>
-    <row r="441" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A441" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2001162111</v>
@@ -45316,9 +45356,11 @@
         <v>11</v>
       </c>
       <c r="I441" s="4"/>
-      <c r="J441" s="7"/>
-    </row>
-    <row r="442" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J441" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A442" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2001272112</v>
@@ -45345,9 +45387,11 @@
         <v>12</v>
       </c>
       <c r="I442" s="4"/>
-      <c r="J442" s="7"/>
-    </row>
-    <row r="443" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J442" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A443" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2002242.5212</v>
@@ -45376,7 +45420,7 @@
       <c r="I443" s="4"/>
       <c r="J443" s="7"/>
     </row>
-    <row r="444" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A444" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2003251.5213</v>
@@ -45405,7 +45449,7 @@
       <c r="I444" s="4"/>
       <c r="J444" s="7"/>
     </row>
-    <row r="445" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A445" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2003262314</v>
@@ -45434,7 +45478,7 @@
       <c r="I445" s="4"/>
       <c r="J445" s="7"/>
     </row>
-    <row r="446" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A446" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2003274.5314</v>
@@ -45463,7 +45507,7 @@
       <c r="I446" s="4"/>
       <c r="J446" s="7"/>
     </row>
-    <row r="447" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A447" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2004154415</v>
@@ -45492,7 +45536,7 @@
       <c r="I447" s="4"/>
       <c r="J447" s="7"/>
     </row>
-    <row r="448" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A448" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2004163416</v>
@@ -45521,7 +45565,7 @@
       <c r="I448" s="4"/>
       <c r="J448" s="7"/>
     </row>
-    <row r="449" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A449" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam2004171416</v>
@@ -45550,7 +45594,7 @@
       <c r="I449" s="4"/>
       <c r="J449" s="7"/>
     </row>
-    <row r="450" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A450" s="7" t="str">
         <f t="shared" si="6"/>
         <v>SectionB_Exam200591517</v>
@@ -45579,7 +45623,7 @@
       <c r="I450" s="4"/>
       <c r="J450" s="7"/>
     </row>
-    <row r="451" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A451" s="7" t="str">
         <f t="shared" ref="A451:A514" si="7">B451&amp;D451&amp;E451&amp;F451&amp;G451&amp;H451</f>
         <v>SectionB_Exam2005141517</v>
@@ -45608,7 +45652,7 @@
       <c r="I451" s="4"/>
       <c r="J451" s="7"/>
     </row>
-    <row r="452" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A452" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam2006111517</v>
@@ -45637,7 +45681,7 @@
       <c r="I452" s="4"/>
       <c r="J452" s="7"/>
     </row>
-    <row r="453" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A453" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam2006123517</v>
@@ -45666,7 +45710,7 @@
       <c r="I453" s="4"/>
       <c r="J453" s="7"/>
     </row>
-    <row r="454" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A454" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam2007102518</v>
@@ -45695,7 +45739,7 @@
       <c r="I454" s="4"/>
       <c r="J454" s="7"/>
     </row>
-    <row r="455" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A455" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam2008122619</v>
@@ -45724,7 +45768,7 @@
       <c r="I455" s="4"/>
       <c r="J455" s="7"/>
     </row>
-    <row r="456" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A456" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam200961.25619</v>
@@ -45753,7 +45797,7 @@
       <c r="I456" s="4"/>
       <c r="J456" s="7"/>
     </row>
-    <row r="457" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A457" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam200992.25620</v>
@@ -45782,7 +45826,7 @@
       <c r="I457" s="4"/>
       <c r="J457" s="7"/>
     </row>
-    <row r="458" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A458" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam2009102720</v>
@@ -45811,7 +45855,7 @@
       <c r="I458" s="4"/>
       <c r="J458" s="7"/>
     </row>
-    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A459" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201071.5721</v>
@@ -45840,7 +45884,7 @@
       <c r="I459" s="4"/>
       <c r="J459" s="7"/>
     </row>
-    <row r="460" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A460" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201222822</v>
@@ -45869,7 +45913,7 @@
       <c r="I460" s="4"/>
       <c r="J460" s="7"/>
     </row>
-    <row r="461" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A461" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201361.5823</v>
@@ -45898,7 +45942,7 @@
       <c r="I461" s="4"/>
       <c r="J461" s="7"/>
     </row>
-    <row r="462" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A462" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201471.5924</v>
@@ -45927,7 +45971,7 @@
       <c r="I462" s="4"/>
       <c r="J462" s="7"/>
     </row>
-    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A463" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201482925</v>
@@ -45956,7 +46000,7 @@
       <c r="I463" s="4"/>
       <c r="J463" s="7"/>
     </row>
-    <row r="464" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A464" s="7" t="str">
         <f t="shared" si="7"/>
         <v>SectionB_Exam201582.751026</v>
@@ -53394,10 +53438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53510,6 +53554,68 @@
         <v>108</v>
       </c>
       <c r="C15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
         <v>109</v>
       </c>
     </row>
@@ -53522,11 +53628,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="W38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="Y56" sqref="Y56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55672,7 +55778,7 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <f t="shared" ref="M56:Y56" si="6">M52-M54</f>
+        <f t="shared" ref="M56:X56" si="6">M52-M54</f>
         <v>0</v>
       </c>
       <c r="N56">

</xml_diff>

<commit_message>
update plan less stressful for upcomeing busy time
</commit_message>
<xml_diff>
--- a/StudyProgress.xlsx
+++ b/StudyProgress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="18180" windowHeight="7152" activeTab="2"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="18180" windowHeight="7152" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RawQuestionDB" sheetId="1" r:id="rId1"/>
@@ -53440,7 +53440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -53628,11 +53628,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="W38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="AA36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y56" sqref="Y56"/>
+      <selection pane="bottomRight" activeCell="AA58" sqref="AA58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53945,11 +53945,14 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>-0.25</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -54176,14 +54179,17 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>2.5666666666666669</v>
+        <v>1.5666666666666669</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
+      <c r="X12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -55353,11 +55359,11 @@
       </c>
       <c r="F52">
         <f>SUM(F2:F51)</f>
-        <v>29.25</v>
+        <v>31.25</v>
       </c>
       <c r="G52">
         <f>E52-F52</f>
-        <v>92.8</v>
+        <v>90.8</v>
       </c>
       <c r="H52">
         <f>SUM(H2:H51)</f>
@@ -55365,7 +55371,7 @@
       </c>
       <c r="I52">
         <f t="shared" ref="I52:AT52" si="5">SUM(I2:I51)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52">
         <f t="shared" si="5"/>
@@ -55425,7 +55431,7 @@
       </c>
       <c r="X52">
         <f t="shared" si="5"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="Y52">
         <f t="shared" si="5"/>
@@ -55525,15 +55531,15 @@
       </c>
       <c r="E54">
         <f>SUM(H54:XFD54)</f>
-        <v>178.5</v>
+        <v>173.75</v>
       </c>
       <c r="F54">
         <f>SUM(H52:AT52)</f>
-        <v>29.25</v>
+        <v>31.25</v>
       </c>
       <c r="G54">
         <f>E54-F54</f>
-        <v>149.25</v>
+        <v>142.5</v>
       </c>
       <c r="H54">
         <v>1.5</v>
@@ -55587,43 +55593,43 @@
         <v>3</v>
       </c>
       <c r="Y54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z54">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AA54">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB54">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AC54">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AD54">
         <v>1.5</v>
       </c>
       <c r="AE54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AH54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ54">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="AK54">
-        <v>1.5</v>
+        <v>3.75</v>
       </c>
       <c r="AL54">
         <v>3</v>
@@ -55644,13 +55650,13 @@
         <v>3</v>
       </c>
       <c r="AR54">
-        <v>1.5</v>
+        <v>3.75</v>
       </c>
       <c r="AS54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AT54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU54">
         <v>3</v>
@@ -55746,7 +55752,7 @@
       </c>
       <c r="E55">
         <f>SUM(H52:BA52)</f>
-        <v>29.25</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.3">
@@ -55755,7 +55761,7 @@
       </c>
       <c r="E56">
         <f>SUM(H56:XFD56)</f>
-        <v>-3.75</v>
+        <v>-1.75</v>
       </c>
       <c r="H56">
         <f>H52-H54</f>
@@ -55763,7 +55769,7 @@
       </c>
       <c r="I56">
         <f>I52-I54</f>
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="J56">
         <f>J52-J54</f>
@@ -55823,7 +55829,7 @@
       </c>
       <c r="X56" s="10">
         <f t="shared" si="6"/>
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="Y56" s="10"/>
     </row>
@@ -55833,7 +55839,7 @@
       </c>
       <c r="G58">
         <f>SUM(H58:XFD58)</f>
-        <v>4</v>
+        <v>24.25</v>
       </c>
       <c r="O58">
         <v>1</v>
@@ -55846,6 +55852,42 @@
       </c>
       <c r="T58">
         <v>1</v>
+      </c>
+      <c r="Z58">
+        <v>1</v>
+      </c>
+      <c r="AA58">
+        <v>1</v>
+      </c>
+      <c r="AB58">
+        <v>1</v>
+      </c>
+      <c r="AC58">
+        <v>1</v>
+      </c>
+      <c r="AD58">
+        <v>1</v>
+      </c>
+      <c r="AJ58">
+        <v>3.75</v>
+      </c>
+      <c r="AK58">
+        <v>3.75</v>
+      </c>
+      <c r="AN58">
+        <v>1</v>
+      </c>
+      <c r="AO58">
+        <v>1</v>
+      </c>
+      <c r="AP58">
+        <v>1</v>
+      </c>
+      <c r="AQ58">
+        <v>1</v>
+      </c>
+      <c r="AR58">
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>